<commit_message>
ported preprocessing script from matlab
</commit_message>
<xml_diff>
--- a/FOAM/Invariant-based/input/FoamData.xlsx
+++ b/FOAM/Invariant-based/input/FoamData.xlsx
@@ -13,12 +13,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="12" uniqueCount="12">
   <si>
     <t>leap-comten-stretch</t>
   </si>
   <si>
     <t>leap-comten-stress</t>
+  </si>
+  <si>
+    <t>leap-comten-stddev</t>
   </si>
   <si>
     <t>leap-shr-strain</t>
@@ -27,16 +30,25 @@
     <t>leap-shr-stress</t>
   </si>
   <si>
+    <t>leap-shr-stddev</t>
+  </si>
+  <si>
     <t>turbo-comten-stretch</t>
   </si>
   <si>
     <t>turbo-comten-stress</t>
   </si>
   <si>
+    <t>turbo-comten-stddev</t>
+  </si>
+  <si>
     <t>turbo-shr-strain</t>
   </si>
   <si>
     <t>turbo-shr-stress</t>
+  </si>
+  <si>
+    <t>turbo-shr-stddev</t>
   </si>
 </sst>
 </file>
@@ -82,7 +94,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -90,12 +102,16 @@
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="true"/>
     <col min="2" max="2" width="18.28515625" customWidth="true"/>
-    <col min="3" max="3" width="14.140625" customWidth="true"/>
-    <col min="4" max="4" width="14.42578125" customWidth="true"/>
-    <col min="5" max="5" width="20.28515625" customWidth="true"/>
-    <col min="6" max="6" width="19.28515625" customWidth="true"/>
-    <col min="7" max="7" width="15.140625" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" customWidth="true"/>
+    <col min="3" max="3" width="19.140625" customWidth="true"/>
+    <col min="4" max="4" width="14.140625" customWidth="true"/>
+    <col min="5" max="5" width="14.42578125" customWidth="true"/>
+    <col min="6" max="6" width="15.140625" customWidth="true"/>
+    <col min="7" max="7" width="20.28515625" customWidth="true"/>
+    <col min="8" max="8" width="19.28515625" customWidth="true"/>
+    <col min="9" max="9" width="20.140625" customWidth="true"/>
+    <col min="10" max="10" width="15.140625" customWidth="true"/>
+    <col min="11" max="11" width="15.28515625" customWidth="true"/>
+    <col min="12" max="12" width="16.140625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -123,6 +139,18 @@
       <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
@@ -132,22 +160,34 @@
         <v>-240.39371509262341</v>
       </c>
       <c r="C2" s="0">
+        <v>15.097489467095883</v>
+      </c>
+      <c r="D2" s="0">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="D2" s="0">
+      <c r="E2" s="0">
         <v>-19.136316158898858</v>
       </c>
-      <c r="E2" s="0">
+      <c r="F2" s="0">
+        <v>4.608429243371674</v>
+      </c>
+      <c r="G2" s="0">
         <v>0.40000000000000002</v>
       </c>
-      <c r="F2" s="0">
+      <c r="H2" s="0">
         <v>-303.62562714997335</v>
       </c>
-      <c r="G2" s="0">
+      <c r="I2" s="0">
+        <v>21.740023283539553</v>
+      </c>
+      <c r="J2" s="0">
         <v>-0.14999999999999999</v>
       </c>
-      <c r="H2" s="0">
+      <c r="K2" s="0">
         <v>-35.413801042127886</v>
+      </c>
+      <c r="L2" s="0">
+        <v>3.3464822952409774</v>
       </c>
     </row>
     <row r="3">
@@ -158,22 +198,34 @@
         <v>-190.26665487849283</v>
       </c>
       <c r="C3" s="0">
+        <v>11.06285366598958</v>
+      </c>
+      <c r="D3" s="0">
         <v>-0.13749999999999998</v>
       </c>
-      <c r="D3" s="0">
+      <c r="E3" s="0">
         <v>-17.285802378211393</v>
       </c>
-      <c r="E3" s="0">
+      <c r="F3" s="0">
+        <v>4.1074277336940925</v>
+      </c>
+      <c r="G3" s="0">
         <v>0.45000000000000007</v>
       </c>
-      <c r="F3" s="0">
+      <c r="H3" s="0">
         <v>-234.64166600794866</v>
       </c>
-      <c r="G3" s="0">
+      <c r="I3" s="0">
+        <v>16.340655996448163</v>
+      </c>
+      <c r="J3" s="0">
         <v>-0.13749999999999998</v>
       </c>
-      <c r="H3" s="0">
+      <c r="K3" s="0">
         <v>-32.03338994853894</v>
+      </c>
+      <c r="L3" s="0">
+        <v>3.0840162020184199</v>
       </c>
     </row>
     <row r="4">
@@ -184,22 +236,34 @@
         <v>-154.90787088989586</v>
       </c>
       <c r="C4" s="0">
+        <v>9.3308004066603125</v>
+      </c>
+      <c r="D4" s="0">
         <v>-0.125</v>
       </c>
-      <c r="D4" s="0">
+      <c r="E4" s="0">
         <v>-15.433371525767843</v>
       </c>
-      <c r="E4" s="0">
+      <c r="F4" s="0">
+        <v>3.6141336427657809</v>
+      </c>
+      <c r="G4" s="0">
         <v>0.5</v>
       </c>
-      <c r="F4" s="0">
+      <c r="H4" s="0">
         <v>-187.63784904666826</v>
       </c>
-      <c r="G4" s="0">
+      <c r="I4" s="0">
+        <v>12.80521277153915</v>
+      </c>
+      <c r="J4" s="0">
         <v>-0.125</v>
       </c>
-      <c r="H4" s="0">
+      <c r="K4" s="0">
         <v>-28.689455390832922</v>
+      </c>
+      <c r="L4" s="0">
+        <v>2.790968772497326</v>
       </c>
     </row>
     <row r="5">
@@ -210,22 +274,34 @@
         <v>-127.95478995421865</v>
       </c>
       <c r="C5" s="0">
+        <v>8.3363727682088342</v>
+      </c>
+      <c r="D5" s="0">
         <v>-0.11249999999999999</v>
       </c>
-      <c r="D5" s="0">
+      <c r="E5" s="0">
         <v>-13.669049216183115</v>
       </c>
-      <c r="E5" s="0">
+      <c r="F5" s="0">
+        <v>3.1764906682497052</v>
+      </c>
+      <c r="G5" s="0">
         <v>0.55000000000000004</v>
       </c>
-      <c r="F5" s="0">
+      <c r="H5" s="0">
         <v>-153.15503617282505</v>
       </c>
-      <c r="G5" s="0">
+      <c r="I5" s="0">
+        <v>10.572153456429737</v>
+      </c>
+      <c r="J5" s="0">
         <v>-0.11249999999999999</v>
       </c>
-      <c r="H5" s="0">
+      <c r="K5" s="0">
         <v>-25.468838633134851</v>
+      </c>
+      <c r="L5" s="0">
+        <v>2.537677303663437</v>
       </c>
     </row>
     <row r="6">
@@ -236,22 +312,34 @@
         <v>-107.01387143143764</v>
       </c>
       <c r="C6" s="0">
+        <v>7.680995997558913</v>
+      </c>
+      <c r="D6" s="0">
         <v>-0.099999999999999992</v>
       </c>
-      <c r="D6" s="0">
+      <c r="E6" s="0">
         <v>-11.970867447717103</v>
       </c>
-      <c r="E6" s="0">
+      <c r="F6" s="0">
+        <v>2.7556625189233235</v>
+      </c>
+      <c r="G6" s="0">
         <v>0.60000000000000009</v>
       </c>
-      <c r="F6" s="0">
+      <c r="H6" s="0">
         <v>-126.91584853742566</v>
       </c>
-      <c r="G6" s="0">
+      <c r="I6" s="0">
+        <v>9.0907733841948879</v>
+      </c>
+      <c r="J6" s="0">
         <v>-0.099999999999999992</v>
       </c>
-      <c r="H6" s="0">
+      <c r="K6" s="0">
         <v>-22.346227153676214</v>
+      </c>
+      <c r="L6" s="0">
+        <v>2.2611042677427968</v>
       </c>
     </row>
     <row r="7">
@@ -262,22 +350,34 @@
         <v>-90.175989374839233</v>
       </c>
       <c r="C7" s="0">
+        <v>7.3469435497430133</v>
+      </c>
+      <c r="D7" s="0">
         <v>-0.087500000000000008</v>
       </c>
-      <c r="D7" s="0">
+      <c r="E7" s="0">
         <v>-10.335049625128985</v>
       </c>
-      <c r="E7" s="0">
+      <c r="F7" s="0">
+        <v>2.3592263727554137</v>
+      </c>
+      <c r="G7" s="0">
         <v>0.64999999999999991</v>
       </c>
-      <c r="F7" s="0">
+      <c r="H7" s="0">
         <v>-106.11493231306737</v>
       </c>
-      <c r="G7" s="0">
+      <c r="I7" s="0">
+        <v>8.007594680186866</v>
+      </c>
+      <c r="J7" s="0">
         <v>-0.087500000000000008</v>
       </c>
-      <c r="H7" s="0">
+      <c r="K7" s="0">
         <v>-19.325726723861372</v>
+      </c>
+      <c r="L7" s="0">
+        <v>1.983490867262176</v>
       </c>
     </row>
     <row r="8">
@@ -288,22 +388,34 @@
         <v>-76.200325177993648</v>
       </c>
       <c r="C8" s="0">
+        <v>6.9468653581294975</v>
+      </c>
+      <c r="D8" s="0">
         <v>-0.074999999999999997</v>
       </c>
-      <c r="D8" s="0">
+      <c r="E8" s="0">
         <v>-8.764959319920905</v>
       </c>
-      <c r="E8" s="0">
+      <c r="F8" s="0">
+        <v>1.9816979647727515</v>
+      </c>
+      <c r="G8" s="0">
         <v>0.69999999999999996</v>
       </c>
-      <c r="F8" s="0">
+      <c r="H8" s="0">
         <v>-89.275676792077235</v>
       </c>
-      <c r="G8" s="0">
+      <c r="I8" s="0">
+        <v>7.2648087450191845</v>
+      </c>
+      <c r="J8" s="0">
         <v>-0.074999999999999997</v>
       </c>
-      <c r="H8" s="0">
+      <c r="K8" s="0">
         <v>-16.393015126993173</v>
+      </c>
+      <c r="L8" s="0">
+        <v>1.7076946700141613</v>
       </c>
     </row>
     <row r="9">
@@ -314,22 +426,34 @@
         <v>-64.535772281428365</v>
       </c>
       <c r="C9" s="0">
+        <v>6.6939585258530165</v>
+      </c>
+      <c r="D9" s="0">
         <v>-0.0625</v>
       </c>
-      <c r="D9" s="0">
+      <c r="E9" s="0">
         <v>-7.2360916886332385</v>
       </c>
-      <c r="E9" s="0">
+      <c r="F9" s="0">
+        <v>1.6195961992862407</v>
+      </c>
+      <c r="G9" s="0">
         <v>0.75</v>
       </c>
-      <c r="F9" s="0">
+      <c r="H9" s="0">
         <v>-75.241770240982333</v>
       </c>
-      <c r="G9" s="0">
+      <c r="I9" s="0">
+        <v>6.7367362287146477</v>
+      </c>
+      <c r="J9" s="0">
         <v>-0.0625</v>
       </c>
-      <c r="H9" s="0">
+      <c r="K9" s="0">
         <v>-13.544355073119551</v>
+      </c>
+      <c r="L9" s="0">
+        <v>1.4331108275587408</v>
       </c>
     </row>
     <row r="10">
@@ -340,22 +464,34 @@
         <v>-54.469522915615158</v>
       </c>
       <c r="C10" s="0">
+        <v>6.4159546688654956</v>
+      </c>
+      <c r="D10" s="0">
         <v>-0.049999999999999996</v>
       </c>
-      <c r="D10" s="0">
+      <c r="E10" s="0">
         <v>-5.746584542048895</v>
       </c>
-      <c r="E10" s="0">
+      <c r="F10" s="0">
+        <v>1.2793083702544212</v>
+      </c>
+      <c r="G10" s="0">
         <v>0.80000000000000004</v>
       </c>
-      <c r="F10" s="0">
+      <c r="H10" s="0">
         <v>-62.800268285288951</v>
       </c>
-      <c r="G10" s="0">
+      <c r="I10" s="0">
+        <v>6.0626554348619086</v>
+      </c>
+      <c r="J10" s="0">
         <v>-0.049999999999999996</v>
       </c>
-      <c r="H10" s="0">
+      <c r="K10" s="0">
         <v>-10.758580520422859</v>
+      </c>
+      <c r="L10" s="0">
+        <v>1.1514166759941995</v>
       </c>
     </row>
     <row r="11">
@@ -366,22 +502,34 @@
         <v>-44.743637705754615</v>
       </c>
       <c r="C11" s="0">
+        <v>5.9971222204372694</v>
+      </c>
+      <c r="D11" s="0">
         <v>-0.037499999999999999</v>
       </c>
-      <c r="D11" s="0">
+      <c r="E11" s="0">
         <v>-4.2875172657388303</v>
       </c>
-      <c r="E11" s="0">
+      <c r="F11" s="0">
+        <v>0.95175752586256335</v>
+      </c>
+      <c r="G11" s="0">
         <v>0.84999999999999998</v>
       </c>
-      <c r="F11" s="0">
+      <c r="H11" s="0">
         <v>-49.843734628596948</v>
       </c>
-      <c r="G11" s="0">
+      <c r="I11" s="0">
+        <v>4.6629921695403196</v>
+      </c>
+      <c r="J11" s="0">
         <v>-0.037499999999999999</v>
       </c>
-      <c r="H11" s="0">
+      <c r="K11" s="0">
         <v>-8.0317613133000147</v>
+      </c>
+      <c r="L11" s="0">
+        <v>0.86485886477362584</v>
       </c>
     </row>
     <row r="12">
@@ -392,22 +540,34 @@
         <v>-31.711658993691465</v>
       </c>
       <c r="C12" s="0">
+        <v>4.3195436863168588</v>
+      </c>
+      <c r="D12" s="0">
         <v>-0.024999999999999998</v>
       </c>
-      <c r="D12" s="0">
+      <c r="E12" s="0">
         <v>-2.8481581211425788</v>
       </c>
-      <c r="E12" s="0">
+      <c r="F12" s="0">
+        <v>0.62854526034693403</v>
+      </c>
+      <c r="G12" s="0">
         <v>0.90000000000000002</v>
       </c>
-      <c r="F12" s="0">
+      <c r="H12" s="0">
         <v>-31.34265474267697</v>
       </c>
-      <c r="G12" s="0">
+      <c r="I12" s="0">
+        <v>1.9763068023580079</v>
+      </c>
+      <c r="J12" s="0">
         <v>-0.024999999999999998</v>
       </c>
-      <c r="H12" s="0">
+      <c r="K12" s="0">
         <v>-5.3344338213995766</v>
+      </c>
+      <c r="L12" s="0">
+        <v>0.58026694833896775</v>
       </c>
     </row>
     <row r="13">
@@ -418,22 +578,34 @@
         <v>-12.178708952942994</v>
       </c>
       <c r="C13" s="0">
+        <v>1.3071418756329023</v>
+      </c>
+      <c r="D13" s="0">
         <v>-0.012499999999999999</v>
       </c>
-      <c r="D13" s="0">
+      <c r="E13" s="0">
         <v>-1.4216968871130082</v>
       </c>
-      <c r="E13" s="0">
+      <c r="F13" s="0">
+        <v>0.31423266369073305</v>
+      </c>
+      <c r="G13" s="0">
         <v>0.94999999999999996</v>
       </c>
-      <c r="F13" s="0">
+      <c r="H13" s="0">
         <v>-8.7113251340128777</v>
       </c>
-      <c r="G13" s="0">
+      <c r="I13" s="0">
+        <v>1.1026942374965207</v>
+      </c>
+      <c r="J13" s="0">
         <v>-0.012499999999999999</v>
       </c>
-      <c r="H13" s="0">
+      <c r="K13" s="0">
         <v>-2.6609549495120186</v>
+      </c>
+      <c r="L13" s="0">
+        <v>0.29133315470443222</v>
       </c>
     </row>
     <row r="14">
@@ -444,22 +616,34 @@
         <v>-0</v>
       </c>
       <c r="C14" s="0">
+        <v>0</v>
+      </c>
+      <c r="D14" s="0">
         <v>-0</v>
       </c>
-      <c r="D14" s="0">
+      <c r="E14" s="0">
         <v>-0.086050826256747176</v>
       </c>
-      <c r="E14" s="0">
+      <c r="F14" s="0">
+        <v>0.019126390667956971</v>
+      </c>
+      <c r="G14" s="0">
         <v>1</v>
       </c>
-      <c r="F14" s="0">
+      <c r="H14" s="0">
         <v>-0</v>
       </c>
-      <c r="G14" s="0">
+      <c r="I14" s="0">
+        <v>0</v>
+      </c>
+      <c r="J14" s="0">
         <v>-0</v>
       </c>
-      <c r="H14" s="0">
+      <c r="K14" s="0">
         <v>-0.1611650062008424</v>
+      </c>
+      <c r="L14" s="0">
+        <v>0.017319591522008911</v>
       </c>
     </row>
     <row r="15">
@@ -470,22 +654,34 @@
         <v>14.192356349932373</v>
       </c>
       <c r="C15" s="0">
+        <v>2.9348496307603043</v>
+      </c>
+      <c r="D15" s="0">
         <v>0.012499999999999999</v>
       </c>
-      <c r="D15" s="0">
+      <c r="E15" s="0">
         <v>1.4216968871130082</v>
       </c>
-      <c r="E15" s="0">
+      <c r="F15" s="0">
+        <v>0.31423266369073305</v>
+      </c>
+      <c r="G15" s="0">
         <v>1.0249999999999999</v>
       </c>
-      <c r="F15" s="0">
+      <c r="H15" s="0">
         <v>16.674089228235811</v>
       </c>
-      <c r="G15" s="0">
+      <c r="I15" s="0">
+        <v>2.7775627544636001</v>
+      </c>
+      <c r="J15" s="0">
         <v>0.012499999999999999</v>
       </c>
-      <c r="H15" s="0">
+      <c r="K15" s="0">
         <v>2.6609549495120186</v>
+      </c>
+      <c r="L15" s="0">
+        <v>0.29133315470443222</v>
       </c>
     </row>
     <row r="16">
@@ -496,22 +692,34 @@
         <v>29.203740088479627</v>
       </c>
       <c r="C16" s="0">
+        <v>6.0262600000492039</v>
+      </c>
+      <c r="D16" s="0">
         <v>0.024999999999999998</v>
       </c>
-      <c r="D16" s="0">
+      <c r="E16" s="0">
         <v>2.8481581211425788</v>
       </c>
-      <c r="E16" s="0">
+      <c r="F16" s="0">
+        <v>0.62854526034693403</v>
+      </c>
+      <c r="G16" s="0">
         <v>1.05</v>
       </c>
-      <c r="F16" s="0">
+      <c r="H16" s="0">
         <v>35.072548340149012</v>
       </c>
-      <c r="G16" s="0">
+      <c r="I16" s="0">
+        <v>5.0844456420560791</v>
+      </c>
+      <c r="J16" s="0">
         <v>0.024999999999999998</v>
       </c>
-      <c r="H16" s="0">
+      <c r="K16" s="0">
         <v>5.3344338213995766</v>
+      </c>
+      <c r="L16" s="0">
+        <v>0.58026694833896775</v>
       </c>
     </row>
     <row r="17">
@@ -522,22 +730,34 @@
         <v>44.788623910602936</v>
       </c>
       <c r="C17" s="0">
+        <v>9.3631495914268541</v>
+      </c>
+      <c r="D17" s="0">
         <v>0.037499999999999999</v>
       </c>
-      <c r="D17" s="0">
+      <c r="E17" s="0">
         <v>4.2875172657388303</v>
       </c>
-      <c r="E17" s="0">
+      <c r="F17" s="0">
+        <v>0.95175752586256335</v>
+      </c>
+      <c r="G17" s="0">
         <v>1.075</v>
       </c>
-      <c r="F17" s="0">
+      <c r="H17" s="0">
         <v>54.485106023345267</v>
       </c>
-      <c r="G17" s="0">
+      <c r="I17" s="0">
+        <v>7.4162859396729148</v>
+      </c>
+      <c r="J17" s="0">
         <v>0.037499999999999999</v>
       </c>
-      <c r="H17" s="0">
+      <c r="K17" s="0">
         <v>8.0317613133000147</v>
+      </c>
+      <c r="L17" s="0">
+        <v>0.86485886477362584</v>
       </c>
     </row>
     <row r="18">
@@ -548,22 +768,34 @@
         <v>61.629267114028167</v>
       </c>
       <c r="C18" s="0">
+        <v>13.149339669410345</v>
+      </c>
+      <c r="D18" s="0">
         <v>0.049999999999999996</v>
       </c>
-      <c r="D18" s="0">
+      <c r="E18" s="0">
         <v>5.746584542048895</v>
       </c>
-      <c r="E18" s="0">
+      <c r="F18" s="0">
+        <v>1.2793083702544212</v>
+      </c>
+      <c r="G18" s="0">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F18" s="0">
+      <c r="H18" s="0">
         <v>75.278149595346235</v>
       </c>
-      <c r="G18" s="0">
+      <c r="I18" s="0">
+        <v>9.7077578054851514</v>
+      </c>
+      <c r="J18" s="0">
         <v>0.049999999999999996</v>
       </c>
-      <c r="H18" s="0">
+      <c r="K18" s="0">
         <v>10.758580520422859</v>
+      </c>
+      <c r="L18" s="0">
+        <v>1.1514166759941995</v>
       </c>
     </row>
     <row r="19">
@@ -574,22 +806,34 @@
         <v>79.567010597536949</v>
       </c>
       <c r="C19" s="0">
+        <v>17.344425610004418</v>
+      </c>
+      <c r="D19" s="0">
         <v>0.0625</v>
       </c>
-      <c r="D19" s="0">
+      <c r="E19" s="0">
         <v>7.2360916886332385</v>
       </c>
-      <c r="E19" s="0">
+      <c r="F19" s="0">
+        <v>1.6195961992862407</v>
+      </c>
+      <c r="G19" s="0">
         <v>1.125</v>
       </c>
-      <c r="F19" s="0">
+      <c r="H19" s="0">
         <v>97.356225341361124</v>
       </c>
-      <c r="G19" s="0">
+      <c r="I19" s="0">
+        <v>11.814652191288889</v>
+      </c>
+      <c r="J19" s="0">
         <v>0.0625</v>
       </c>
-      <c r="H19" s="0">
+      <c r="K19" s="0">
         <v>13.544355073119551</v>
+      </c>
+      <c r="L19" s="0">
+        <v>1.4331108275587408</v>
       </c>
     </row>
     <row r="20">
@@ -600,22 +844,34 @@
         <v>98.238643550347405</v>
       </c>
       <c r="C20" s="0">
+        <v>21.600949168462606</v>
+      </c>
+      <c r="D20" s="0">
         <v>0.074999999999999997</v>
       </c>
-      <c r="D20" s="0">
+      <c r="E20" s="0">
         <v>8.764959319920905</v>
       </c>
-      <c r="E20" s="0">
+      <c r="F20" s="0">
+        <v>1.9816979647727515</v>
+      </c>
+      <c r="G20" s="0">
         <v>1.1499999999999999</v>
       </c>
-      <c r="F20" s="0">
+      <c r="H20" s="0">
         <v>120.57254472688503</v>
       </c>
-      <c r="G20" s="0">
+      <c r="I20" s="0">
+        <v>13.823256861721797</v>
+      </c>
+      <c r="J20" s="0">
         <v>0.074999999999999997</v>
       </c>
-      <c r="H20" s="0">
+      <c r="K20" s="0">
         <v>16.393015126993173</v>
+      </c>
+      <c r="L20" s="0">
+        <v>1.7076946700141613</v>
       </c>
     </row>
     <row r="21">
@@ -626,22 +882,34 @@
         <v>117.33246618555684</v>
       </c>
       <c r="C21" s="0">
+        <v>25.71580170945969</v>
+      </c>
+      <c r="D21" s="0">
         <v>0.087500000000000008</v>
       </c>
-      <c r="D21" s="0">
+      <c r="E21" s="0">
         <v>10.335049625128985</v>
       </c>
-      <c r="E21" s="0">
+      <c r="F21" s="0">
+        <v>2.3592263727554137</v>
+      </c>
+      <c r="G21" s="0">
         <v>1.175</v>
       </c>
-      <c r="F21" s="0">
+      <c r="H21" s="0">
         <v>144.68234537680345</v>
       </c>
-      <c r="G21" s="0">
+      <c r="I21" s="0">
+        <v>15.582148705950029</v>
+      </c>
+      <c r="J21" s="0">
         <v>0.087500000000000008</v>
       </c>
-      <c r="H21" s="0">
+      <c r="K21" s="0">
         <v>19.325726723861372</v>
+      </c>
+      <c r="L21" s="0">
+        <v>1.983490867262176</v>
       </c>
     </row>
     <row r="22">
@@ -652,22 +920,34 @@
         <v>136.60924582863572</v>
       </c>
       <c r="C22" s="0">
+        <v>29.550984829753752</v>
+      </c>
+      <c r="D22" s="0">
         <v>0.099999999999999992</v>
       </c>
-      <c r="D22" s="0">
+      <c r="E22" s="0">
         <v>11.970867447717103</v>
       </c>
-      <c r="E22" s="0">
+      <c r="F22" s="0">
+        <v>2.7556625189233235</v>
+      </c>
+      <c r="G22" s="0">
         <v>1.2</v>
       </c>
-      <c r="F22" s="0">
+      <c r="H22" s="0">
         <v>169.49710255058815</v>
       </c>
-      <c r="G22" s="0">
+      <c r="I22" s="0">
+        <v>17.243625411440192</v>
+      </c>
+      <c r="J22" s="0">
         <v>0.099999999999999992</v>
       </c>
-      <c r="H22" s="0">
+      <c r="K22" s="0">
         <v>22.346227153676214</v>
+      </c>
+      <c r="L22" s="0">
+        <v>2.2611042677427968</v>
       </c>
     </row>
     <row r="23">
@@ -678,22 +958,34 @@
         <v>155.79071305113351</v>
       </c>
       <c r="C23" s="0">
+        <v>32.993340922545265</v>
+      </c>
+      <c r="D23" s="0">
         <v>0.11249999999999999</v>
       </c>
-      <c r="D23" s="0">
+      <c r="E23" s="0">
         <v>13.669049216183115</v>
       </c>
-      <c r="E23" s="0">
+      <c r="F23" s="0">
+        <v>3.1764906682497052</v>
+      </c>
+      <c r="G23" s="0">
         <v>1.2250000000000001</v>
       </c>
-      <c r="F23" s="0">
+      <c r="H23" s="0">
         <v>194.60682878232228</v>
       </c>
-      <c r="G23" s="0">
+      <c r="I23" s="0">
+        <v>18.95418606582281</v>
+      </c>
+      <c r="J23" s="0">
         <v>0.11249999999999999</v>
       </c>
-      <c r="H23" s="0">
+      <c r="K23" s="0">
         <v>25.468838633134851</v>
+      </c>
+      <c r="L23" s="0">
+        <v>2.537677303663437</v>
       </c>
     </row>
     <row r="24">
@@ -704,22 +996,34 @@
         <v>174.71894219523253</v>
       </c>
       <c r="C24" s="0">
+        <v>36.016518571080091</v>
+      </c>
+      <c r="D24" s="0">
         <v>0.125</v>
       </c>
-      <c r="D24" s="0">
+      <c r="E24" s="0">
         <v>15.433371525767843</v>
       </c>
-      <c r="E24" s="0">
+      <c r="F24" s="0">
+        <v>3.6141336427657809</v>
+      </c>
+      <c r="G24" s="0">
         <v>1.25</v>
       </c>
-      <c r="F24" s="0">
+      <c r="H24" s="0">
         <v>219.66424270723184</v>
       </c>
-      <c r="G24" s="0">
+      <c r="I24" s="0">
+        <v>20.582624661537437</v>
+      </c>
+      <c r="J24" s="0">
         <v>0.125</v>
       </c>
-      <c r="H24" s="0">
+      <c r="K24" s="0">
         <v>28.689455390832922</v>
+      </c>
+      <c r="L24" s="0">
+        <v>2.790968772497326</v>
       </c>
     </row>
     <row r="25">
@@ -730,22 +1034,34 @@
         <v>193.25811195370036</v>
       </c>
       <c r="C25" s="0">
+        <v>38.723269659990933</v>
+      </c>
+      <c r="D25" s="0">
         <v>0.13749999999999998</v>
       </c>
-      <c r="D25" s="0">
+      <c r="E25" s="0">
         <v>17.285802378211393</v>
       </c>
-      <c r="E25" s="0">
+      <c r="F25" s="0">
+        <v>4.1074277336940925</v>
+      </c>
+      <c r="G25" s="0">
         <v>1.2749999999999999</v>
       </c>
-      <c r="F25" s="0">
+      <c r="H25" s="0">
         <v>244.41974414685842</v>
       </c>
-      <c r="G25" s="0">
+      <c r="I25" s="0">
+        <v>22.046181546046707</v>
+      </c>
+      <c r="J25" s="0">
         <v>0.13749999999999998</v>
       </c>
-      <c r="H25" s="0">
+      <c r="K25" s="0">
         <v>32.03338994853894</v>
+      </c>
+      <c r="L25" s="0">
+        <v>3.0840162020184199</v>
       </c>
     </row>
     <row r="26">
@@ -756,22 +1072,34 @@
         <v>211.48027387477259</v>
       </c>
       <c r="C26" s="0">
+        <v>41.108593983572227</v>
+      </c>
+      <c r="D26" s="0">
         <v>0.14999999999999999</v>
       </c>
-      <c r="D26" s="0">
+      <c r="E26" s="0">
         <v>19.136316158898858</v>
       </c>
-      <c r="E26" s="0">
+      <c r="F26" s="0">
+        <v>4.608429243371674</v>
+      </c>
+      <c r="G26" s="0">
         <v>1.3</v>
       </c>
-      <c r="F26" s="0">
+      <c r="H26" s="0">
         <v>268.84598073948717</v>
       </c>
-      <c r="G26" s="0">
+      <c r="I26" s="0">
+        <v>23.415231872983494</v>
+      </c>
+      <c r="J26" s="0">
         <v>0.14999999999999999</v>
       </c>
-      <c r="H26" s="0">
+      <c r="K26" s="0">
         <v>35.413801042127886</v>
+      </c>
+      <c r="L26" s="0">
+        <v>3.3464822952409774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>